<commit_message>
solicitud de cambios y documentación de cambios
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/01. Requerimientos/ControlDeGastos-Estimacion.xlsx
+++ b/Proyectos/ControlDeGastos/01. Requerimientos/ControlDeGastos-Estimacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DescripcionesInstrucciones" sheetId="1" state="visible" r:id="rId2"/>
@@ -585,7 +585,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
   <si>
     <t>Descripción / Instrucciones</t>
   </si>
@@ -918,6 +918,9 @@
     <t>Cambios</t>
   </si>
   <si>
+    <t>Permitir cambiar los gastos a diferentes tipos de cuentas</t>
+  </si>
+  <si>
     <t>Sueldo Base</t>
   </si>
   <si>
@@ -1108,7 +1111,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7F7F7F"/>
-        <bgColor rgb="FF96989A"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -1142,7 +1145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1224,6 +1227,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1256,7 +1270,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1605,12 +1619,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1648,11 +1666,11 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFBFBFBF"/>
-      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FFA6A6A6"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1703,15 +1721,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1947960</xdr:colOff>
+      <xdr:colOff>1974960</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2066040</xdr:colOff>
+      <xdr:colOff>2092680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823680</xdr:rowOff>
+      <xdr:rowOff>823320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1724,8 +1742,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3026160" y="0"/>
-          <a:ext cx="2637720" cy="823680"/>
+          <a:off x="3053160" y="0"/>
+          <a:ext cx="2637360" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1745,15 +1763,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>279360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>38520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>824760</xdr:rowOff>
+      <xdr:rowOff>824400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1766,8 +1784,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7911720" y="1080"/>
-          <a:ext cx="2621160" cy="823680"/>
+          <a:off x="7938720" y="1080"/>
+          <a:ext cx="2620800" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1787,15 +1805,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>509760</xdr:colOff>
+      <xdr:colOff>536760</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>842040</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823680</xdr:rowOff>
+      <xdr:rowOff>823320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1808,8 +1826,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6859440" y="0"/>
-          <a:ext cx="2619720" cy="823680"/>
+          <a:off x="6886440" y="0"/>
+          <a:ext cx="2619360" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1829,15 +1847,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>214560</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>761040</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>824760</xdr:rowOff>
+      <xdr:rowOff>824400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1850,8 +1868,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6664680" y="1080"/>
-          <a:ext cx="2612160" cy="823680"/>
+          <a:off x="6691680" y="1080"/>
+          <a:ext cx="2611800" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -51135,7 +51153,7 @@
   </sheetPr>
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -51627,8 +51645,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -51693,16 +51711,16 @@
       </c>
       <c r="C5" s="69" t="n">
         <f aca="false">SUM(C6,C15)</f>
-        <v>97.4075625</v>
+        <v>112.4075625</v>
       </c>
       <c r="D5" s="70" t="n">
         <f aca="false">SUM(D6,D15)</f>
-        <v>6379.509375</v>
+        <v>7504.509375</v>
       </c>
       <c r="E5" s="70"/>
       <c r="F5" s="70" t="n">
         <f aca="false">SUM(F6,F15)</f>
-        <v>8293.3621875</v>
+        <v>9418.3621875</v>
       </c>
       <c r="G5" s="70"/>
     </row>
@@ -51957,16 +51975,16 @@
       </c>
       <c r="C15" s="85" t="n">
         <f aca="false">SUM(C17:C19)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D15" s="73" t="n">
         <f aca="false">SUM(E17:E19)</f>
-        <v>0</v>
+        <v>1125</v>
       </c>
       <c r="E15" s="73"/>
       <c r="F15" s="73" t="n">
         <f aca="false">SUM(G17:G19)</f>
-        <v>0</v>
+        <v>1125</v>
       </c>
       <c r="G15" s="73"/>
     </row>
@@ -51993,28 +52011,36 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A17" s="86" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="80"/>
+      <c r="B17" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" s="80" t="n">
+        <v>75</v>
+      </c>
       <c r="E17" s="81" t="n">
         <f aca="false">C17*D17</f>
-        <v>0</v>
+        <v>1125</v>
       </c>
-      <c r="F17" s="82"/>
+      <c r="F17" s="82" t="n">
+        <v>75</v>
+      </c>
       <c r="G17" s="83" t="n">
         <f aca="false">C17*F17</f>
-        <v>0</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A18" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="87"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="88"/>
       <c r="D18" s="80"/>
       <c r="E18" s="81" t="n">
@@ -52031,7 +52057,7 @@
       <c r="A19" s="86" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="87"/>
+      <c r="B19" s="89"/>
       <c r="C19" s="88"/>
       <c r="D19" s="80"/>
       <c r="E19" s="81" t="n">
@@ -52088,44 +52114,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="89" t="s">
-        <v>105</v>
+      <c r="A2" s="90" t="s">
+        <v>106</v>
       </c>
-      <c r="B2" s="90" t="n">
+      <c r="B2" s="91" t="n">
         <v>12000</v>
       </c>
-      <c r="C2" s="91" t="n">
+      <c r="C2" s="92" t="n">
         <f aca="false">B2/160</f>
         <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
-        <v>106</v>
+      <c r="A3" s="90" t="s">
+        <v>107</v>
       </c>
-      <c r="B3" s="90" t="n">
+      <c r="B3" s="91" t="n">
         <v>10000</v>
       </c>
-      <c r="C3" s="91" t="n">
+      <c r="C3" s="92" t="n">
         <f aca="false">B3/160</f>
         <v>62.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="90" t="n">
+      <c r="B4" s="91" t="n">
         <v>8000</v>
       </c>
-      <c r="C4" s="91" t="n">
+      <c r="C4" s="92" t="n">
         <f aca="false">B4/160</f>
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
revision de documentos necesarios para la elaboración de acciones correctivas, reporte de monitoreo minuta y concentrado de metricas
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/01. Requerimientos/ControlDeGastos-Estimacion.xlsx
+++ b/Proyectos/ControlDeGastos/01. Requerimientos/ControlDeGastos-Estimacion.xlsx
@@ -1721,15 +1721,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1974960</xdr:colOff>
+      <xdr:colOff>2001960</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2092680</xdr:colOff>
+      <xdr:colOff>2119320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823320</xdr:rowOff>
+      <xdr:rowOff>822960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1742,8 +1742,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3053160" y="0"/>
-          <a:ext cx="2637360" cy="823320"/>
+          <a:off x="3080160" y="0"/>
+          <a:ext cx="2637000" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1762,16 +1762,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>279360</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>38520</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>824400</xdr:rowOff>
+      <xdr:rowOff>824040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1784,8 +1784,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7938720" y="1080"/>
-          <a:ext cx="2620800" cy="823320"/>
+          <a:off x="7965720" y="1080"/>
+          <a:ext cx="2620440" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1805,15 +1805,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>536760</xdr:colOff>
+      <xdr:colOff>563760</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
+      <xdr:colOff>38880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823320</xdr:rowOff>
+      <xdr:rowOff>822960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1826,8 +1826,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6886440" y="0"/>
-          <a:ext cx="2619360" cy="823320"/>
+          <a:off x="6913440" y="0"/>
+          <a:ext cx="2619000" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1847,15 +1847,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>21960</xdr:colOff>
+      <xdr:colOff>48600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>824400</xdr:rowOff>
+      <xdr:rowOff>824040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1868,8 +1868,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6691680" y="1080"/>
-          <a:ext cx="2611800" cy="823320"/>
+          <a:off x="6718680" y="1080"/>
+          <a:ext cx="2611440" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -51646,7 +51646,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -51711,16 +51711,16 @@
       </c>
       <c r="C5" s="69" t="n">
         <f aca="false">SUM(C6,C15)</f>
-        <v>112.4075625</v>
+        <v>105.4075625</v>
       </c>
       <c r="D5" s="70" t="n">
         <f aca="false">SUM(D6,D15)</f>
-        <v>7504.509375</v>
+        <v>6979.509375</v>
       </c>
       <c r="E5" s="70"/>
       <c r="F5" s="70" t="n">
         <f aca="false">SUM(F6,F15)</f>
-        <v>9418.3621875</v>
+        <v>8893.3621875</v>
       </c>
       <c r="G5" s="70"/>
     </row>
@@ -51975,16 +51975,16 @@
       </c>
       <c r="C15" s="85" t="n">
         <f aca="false">SUM(C17:C19)</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D15" s="73" t="n">
         <f aca="false">SUM(E17:E19)</f>
-        <v>1125</v>
+        <v>600</v>
       </c>
       <c r="E15" s="73"/>
       <c r="F15" s="73" t="n">
         <f aca="false">SUM(G17:G19)</f>
-        <v>1125</v>
+        <v>600</v>
       </c>
       <c r="G15" s="73"/>
     </row>
@@ -52019,21 +52019,21 @@
         <v>103</v>
       </c>
       <c r="C17" s="88" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D17" s="80" t="n">
         <v>75</v>
       </c>
       <c r="E17" s="81" t="n">
         <f aca="false">C17*D17</f>
-        <v>1125</v>
+        <v>600</v>
       </c>
       <c r="F17" s="82" t="n">
         <v>75</v>
       </c>
       <c r="G17" s="83" t="n">
         <f aca="false">C17*F17</f>
-        <v>1125</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">

</xml_diff>